<commit_message>
Update Combined water budget to include Millennium and recovery and add Powell Release
</commit_message>
<xml_diff>
--- a/Powell10year/Curtailment.xlsx
+++ b/Powell10year/Curtailment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\Powell10year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A85715-AEBD-44CF-8D29-2C08C7D1245C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C60FA16-2DE4-4AB3-AA43-B3D5C8721646}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" xr2:uid="{BB94B92A-C8EF-4BFC-A8C8-F3C66B3235F7}"/>
   </bookViews>
@@ -5074,12 +5074,12 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A3" sqref="A3:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="11.81640625" customWidth="1"/>
     <col min="4" max="4" width="8.6328125" customWidth="1"/>

</xml_diff>